<commit_message>
added engage_analysisv1 for chp testing
</commit_message>
<xml_diff>
--- a/Engage-Testing/structure/geothermal_data.xlsx
+++ b/Engage-Testing/structure/geothermal_data.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bpulluta/python-geophires-x/Engage-Testing/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A63E73F-F0FD-E443-B0AB-3FCB588CC294}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-51200" yWindow="500" windowWidth="25600" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="geothermal_data" sheetId="1" r:id="rId1"/>
+    <sheet r:id="rId1" sheetId="1" name="geothermal_data"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -556,77 +550,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
-      <sz val="12"/>
+      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri Light"/>
-      <family val="2"/>
-      <scheme val="major"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF9C5700"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -634,66 +563,18 @@
     <font>
       <b/>
       <sz val="12"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="12"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="12"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="40">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -702,221 +583,41 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor rgb="FFe2f0d9"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor rgb="FFdeebf7"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor rgb="FFfbe5d6"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor rgb="FFfff2cc"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FFd0cece"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor rgb="FFdae3f3"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFEF9AD9"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FFef9ad9"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -925,240 +626,62 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thick">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thick">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.39997558519241921"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF000000"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF000000"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="39" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+  <cellXfs count="10">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="6" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="7" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="8" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="42">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
+  <cellStyles count="1">
+    <cellStyle xfId="0" builtinId="0" name="Normal"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <mruColors>
-      <color rgb="FFEF9AD9"/>
-    </mruColors>
-  </colors>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1169,10 +692,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -1199,116 +722,82 @@
         <a:srgbClr val="70AD47"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Times New Roman" script="Arab"/>
+        <a:font typeface="Times New Roman" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="MoolBoran" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Times New Roman" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Arial" script="Arab"/>
+        <a:font typeface="Arial" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="DaunPenh" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Arial" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1320,160 +809,183 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="35000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
+                <a:tint val="51000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="80000">
               <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
+                <a:tint val="15000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+                <a:tint val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="9500"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot rev="0" lon="0" lat="0"/>
+            </a:camera>
+            <a:lightRig dir="t" rig="threePt">
+              <a:rot rev="1200000" lon="0" lat="0"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="40000">
               <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:tint val="20000"/>
+                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
   <dimension ref="A1:B182"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="B41" sqref="A41:B41"/>
-    </sheetView>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="41.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" style="9" width="41.71928571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="9" width="40.005" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1481,7 +993,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1489,7 +1001,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -1497,7 +1009,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -1505,7 +1017,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
@@ -1513,7 +1025,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18">
       <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
@@ -1521,7 +1033,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18">
       <c r="A7" s="2" t="s">
         <v>2</v>
       </c>
@@ -1529,7 +1041,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18">
       <c r="A8" s="2" t="s">
         <v>2</v>
       </c>
@@ -1537,7 +1049,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18">
       <c r="A9" s="2" t="s">
         <v>2</v>
       </c>
@@ -1545,7 +1057,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18">
       <c r="A10" s="2" t="s">
         <v>2</v>
       </c>
@@ -1553,7 +1065,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18">
       <c r="A11" s="2" t="s">
         <v>2</v>
       </c>
@@ -1561,7 +1073,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18">
       <c r="A12" s="2" t="s">
         <v>2</v>
       </c>
@@ -1569,7 +1081,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18">
       <c r="A13" s="2" t="s">
         <v>2</v>
       </c>
@@ -1577,7 +1089,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18">
       <c r="A14" s="2" t="s">
         <v>2</v>
       </c>
@@ -1585,7 +1097,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18">
       <c r="A15" s="2" t="s">
         <v>2</v>
       </c>
@@ -1593,7 +1105,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18">
       <c r="A16" s="2" t="s">
         <v>2</v>
       </c>
@@ -1601,7 +1113,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18">
       <c r="A17" s="2" t="s">
         <v>2</v>
       </c>
@@ -1609,7 +1121,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18">
       <c r="A18" s="2" t="s">
         <v>2</v>
       </c>
@@ -1617,7 +1129,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18">
       <c r="A19" s="2" t="s">
         <v>2</v>
       </c>
@@ -1625,7 +1137,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18">
       <c r="A20" s="2" t="s">
         <v>2</v>
       </c>
@@ -1633,7 +1145,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18">
       <c r="A21" s="2" t="s">
         <v>2</v>
       </c>
@@ -1641,7 +1153,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18">
       <c r="A22" s="2" t="s">
         <v>2</v>
       </c>
@@ -1649,7 +1161,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18">
       <c r="A23" s="2" t="s">
         <v>2</v>
       </c>
@@ -1657,7 +1169,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18">
       <c r="A24" s="2" t="s">
         <v>2</v>
       </c>
@@ -1665,7 +1177,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18">
       <c r="A25" s="2" t="s">
         <v>2</v>
       </c>
@@ -1673,7 +1185,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18">
       <c r="A26" s="2" t="s">
         <v>2</v>
       </c>
@@ -1681,7 +1193,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18">
       <c r="A27" s="3" t="s">
         <v>28</v>
       </c>
@@ -1689,7 +1201,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18">
       <c r="A28" s="3" t="s">
         <v>28</v>
       </c>
@@ -1697,7 +1209,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18">
       <c r="A29" s="3" t="s">
         <v>28</v>
       </c>
@@ -1705,7 +1217,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18">
       <c r="A30" s="3" t="s">
         <v>28</v>
       </c>
@@ -1713,7 +1225,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18">
       <c r="A31" s="3" t="s">
         <v>28</v>
       </c>
@@ -1721,7 +1233,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18">
       <c r="A32" s="3" t="s">
         <v>28</v>
       </c>
@@ -1729,7 +1241,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18">
       <c r="A33" s="3" t="s">
         <v>28</v>
       </c>
@@ -1737,7 +1249,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18">
       <c r="A34" s="3" t="s">
         <v>28</v>
       </c>
@@ -1745,7 +1257,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18">
       <c r="A35" s="3" t="s">
         <v>28</v>
       </c>
@@ -1753,7 +1265,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18">
       <c r="A36" s="3" t="s">
         <v>28</v>
       </c>
@@ -1761,7 +1273,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18">
       <c r="A37" s="4" t="s">
         <v>39</v>
       </c>
@@ -1769,7 +1281,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18">
       <c r="A38" s="4" t="s">
         <v>39</v>
       </c>
@@ -1777,7 +1289,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18">
       <c r="A39" s="4" t="s">
         <v>39</v>
       </c>
@@ -1785,7 +1297,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18">
       <c r="A40" s="4" t="s">
         <v>39</v>
       </c>
@@ -1793,7 +1305,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="18">
       <c r="A41" s="4" t="s">
         <v>39</v>
       </c>
@@ -1801,7 +1313,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="18">
       <c r="A42" s="4" t="s">
         <v>39</v>
       </c>
@@ -1809,7 +1321,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="18">
       <c r="A43" s="4" t="s">
         <v>39</v>
       </c>
@@ -1817,7 +1329,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="18">
       <c r="A44" s="4" t="s">
         <v>39</v>
       </c>
@@ -1825,7 +1337,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="18">
       <c r="A45" s="4" t="s">
         <v>39</v>
       </c>
@@ -1833,7 +1345,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="18">
       <c r="A46" s="4" t="s">
         <v>39</v>
       </c>
@@ -1841,7 +1353,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="18">
       <c r="A47" s="4" t="s">
         <v>39</v>
       </c>
@@ -1849,7 +1361,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="18">
       <c r="A48" s="4" t="s">
         <v>39</v>
       </c>
@@ -1857,7 +1369,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="18">
       <c r="A49" s="4" t="s">
         <v>39</v>
       </c>
@@ -1865,7 +1377,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="18">
       <c r="A50" s="4" t="s">
         <v>39</v>
       </c>
@@ -1873,7 +1385,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="18">
       <c r="A51" s="4" t="s">
         <v>39</v>
       </c>
@@ -1881,7 +1393,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="18">
       <c r="A52" s="4" t="s">
         <v>39</v>
       </c>
@@ -1889,7 +1401,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="18">
       <c r="A53" s="4" t="s">
         <v>39</v>
       </c>
@@ -1897,7 +1409,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="18">
       <c r="A54" s="4" t="s">
         <v>39</v>
       </c>
@@ -1905,7 +1417,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="18">
       <c r="A55" s="4" t="s">
         <v>39</v>
       </c>
@@ -1913,7 +1425,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="18">
       <c r="A56" s="4" t="s">
         <v>39</v>
       </c>
@@ -1921,7 +1433,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="18">
       <c r="A57" s="4" t="s">
         <v>39</v>
       </c>
@@ -1929,7 +1441,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="18">
       <c r="A58" s="5" t="s">
         <v>57</v>
       </c>
@@ -1937,7 +1449,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="18">
       <c r="A59" s="5" t="s">
         <v>57</v>
       </c>
@@ -1945,7 +1457,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="18">
       <c r="A60" s="5" t="s">
         <v>57</v>
       </c>
@@ -1953,7 +1465,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="18">
       <c r="A61" s="5" t="s">
         <v>57</v>
       </c>
@@ -1961,7 +1473,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="18">
       <c r="A62" s="5" t="s">
         <v>57</v>
       </c>
@@ -1969,7 +1481,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="18">
       <c r="A63" s="5" t="s">
         <v>57</v>
       </c>
@@ -1977,7 +1489,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="18">
       <c r="A64" s="5" t="s">
         <v>57</v>
       </c>
@@ -1985,7 +1497,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="18">
       <c r="A65" s="5" t="s">
         <v>57</v>
       </c>
@@ -1993,7 +1505,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="18">
       <c r="A66" s="5" t="s">
         <v>57</v>
       </c>
@@ -2001,7 +1513,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="18">
       <c r="A67" s="5" t="s">
         <v>57</v>
       </c>
@@ -2009,7 +1521,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="68" customHeight="1" ht="18">
       <c r="A68" s="6" t="s">
         <v>60</v>
       </c>
@@ -2017,7 +1529,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="69" customHeight="1" ht="18">
       <c r="A69" s="6" t="s">
         <v>60</v>
       </c>
@@ -2025,7 +1537,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="70" customHeight="1" ht="18">
       <c r="A70" s="6" t="s">
         <v>60</v>
       </c>
@@ -2033,7 +1545,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="71" customHeight="1" ht="18">
       <c r="A71" s="6" t="s">
         <v>60</v>
       </c>
@@ -2041,7 +1553,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="72" customHeight="1" ht="18">
       <c r="A72" s="6" t="s">
         <v>60</v>
       </c>
@@ -2049,7 +1561,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="73" customHeight="1" ht="18">
       <c r="A73" s="6" t="s">
         <v>60</v>
       </c>
@@ -2057,7 +1569,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="74" customHeight="1" ht="18">
       <c r="A74" s="6" t="s">
         <v>60</v>
       </c>
@@ -2065,7 +1577,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="75" customHeight="1" ht="18">
       <c r="A75" s="6" t="s">
         <v>60</v>
       </c>
@@ -2073,7 +1585,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="76" customHeight="1" ht="18">
       <c r="A76" s="6" t="s">
         <v>60</v>
       </c>
@@ -2081,7 +1593,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="18">
       <c r="A77" s="6" t="s">
         <v>60</v>
       </c>
@@ -2089,7 +1601,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="78" customHeight="1" ht="18">
       <c r="A78" s="6" t="s">
         <v>60</v>
       </c>
@@ -2097,7 +1609,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="79" customHeight="1" ht="18">
       <c r="A79" s="6" t="s">
         <v>60</v>
       </c>
@@ -2105,7 +1617,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="80" customHeight="1" ht="18">
       <c r="A80" s="6" t="s">
         <v>60</v>
       </c>
@@ -2113,7 +1625,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="81" customHeight="1" ht="18">
       <c r="A81" s="6" t="s">
         <v>60</v>
       </c>
@@ -2121,7 +1633,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="82" customHeight="1" ht="18">
       <c r="A82" s="6" t="s">
         <v>60</v>
       </c>
@@ -2129,7 +1641,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="83" customHeight="1" ht="18">
       <c r="A83" s="6" t="s">
         <v>60</v>
       </c>
@@ -2137,7 +1649,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="84" customHeight="1" ht="18">
       <c r="A84" s="6" t="s">
         <v>60</v>
       </c>
@@ -2145,7 +1657,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="85" customHeight="1" ht="18">
       <c r="A85" s="2" t="s">
         <v>78</v>
       </c>
@@ -2153,7 +1665,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="86" customHeight="1" ht="18">
       <c r="A86" s="2" t="s">
         <v>78</v>
       </c>
@@ -2161,7 +1673,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="87" customHeight="1" ht="18">
       <c r="A87" s="2" t="s">
         <v>78</v>
       </c>
@@ -2169,7 +1681,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="88" customHeight="1" ht="18">
       <c r="A88" s="2" t="s">
         <v>78</v>
       </c>
@@ -2177,7 +1689,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="89" customHeight="1" ht="18">
       <c r="A89" s="2" t="s">
         <v>78</v>
       </c>
@@ -2185,7 +1697,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="90" customHeight="1" ht="18">
       <c r="A90" s="2" t="s">
         <v>78</v>
       </c>
@@ -2193,7 +1705,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="91" customHeight="1" ht="18">
       <c r="A91" s="2" t="s">
         <v>78</v>
       </c>
@@ -2201,7 +1713,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="92" customHeight="1" ht="18">
       <c r="A92" s="2" t="s">
         <v>78</v>
       </c>
@@ -2209,7 +1721,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="93" customHeight="1" ht="18">
       <c r="A93" s="2" t="s">
         <v>78</v>
       </c>
@@ -2217,7 +1729,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="94" customHeight="1" ht="20.25">
       <c r="A94" s="2" t="s">
         <v>78</v>
       </c>
@@ -2225,7 +1737,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="95" customHeight="1" ht="18">
       <c r="A95" s="2" t="s">
         <v>78</v>
       </c>
@@ -2233,7 +1745,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="96" customHeight="1" ht="18">
       <c r="A96" s="2" t="s">
         <v>78</v>
       </c>
@@ -2241,7 +1753,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="97" customHeight="1" ht="18">
       <c r="A97" s="2" t="s">
         <v>78</v>
       </c>
@@ -2249,7 +1761,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="98" customHeight="1" ht="18">
       <c r="A98" s="2" t="s">
         <v>78</v>
       </c>
@@ -2257,7 +1769,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="99" customHeight="1" ht="18">
       <c r="A99" s="2" t="s">
         <v>78</v>
       </c>
@@ -2265,7 +1777,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="100" customHeight="1" ht="18">
       <c r="A100" s="2" t="s">
         <v>78</v>
       </c>
@@ -2273,7 +1785,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="101" customHeight="1" ht="18">
       <c r="A101" s="2" t="s">
         <v>78</v>
       </c>
@@ -2281,7 +1793,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="102" customHeight="1" ht="18">
       <c r="A102" s="2" t="s">
         <v>78</v>
       </c>
@@ -2289,7 +1801,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="103" customHeight="1" ht="18">
       <c r="A103" s="2" t="s">
         <v>78</v>
       </c>
@@ -2297,7 +1809,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="104" customHeight="1" ht="18">
       <c r="A104" s="2" t="s">
         <v>78</v>
       </c>
@@ -2305,7 +1817,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="105" customHeight="1" ht="18">
       <c r="A105" s="2" t="s">
         <v>78</v>
       </c>
@@ -2313,7 +1825,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="106" customHeight="1" ht="18">
       <c r="A106" s="2" t="s">
         <v>78</v>
       </c>
@@ -2321,7 +1833,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="107" customHeight="1" ht="18">
       <c r="A107" s="2" t="s">
         <v>78</v>
       </c>
@@ -2329,7 +1841,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="108" customHeight="1" ht="18">
       <c r="A108" s="2" t="s">
         <v>78</v>
       </c>
@@ -2337,7 +1849,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="109" customHeight="1" ht="18">
       <c r="A109" s="2" t="s">
         <v>78</v>
       </c>
@@ -2345,7 +1857,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="110" customHeight="1" ht="18">
       <c r="A110" s="2" t="s">
         <v>78</v>
       </c>
@@ -2353,7 +1865,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="111" customHeight="1" ht="18">
       <c r="A111" s="2" t="s">
         <v>78</v>
       </c>
@@ -2361,7 +1873,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="112" customHeight="1" ht="18">
       <c r="A112" s="2" t="s">
         <v>78</v>
       </c>
@@ -2369,7 +1881,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="113" customHeight="1" ht="18">
       <c r="A113" s="4" t="s">
         <v>106</v>
       </c>
@@ -2377,7 +1889,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="114" customHeight="1" ht="18">
       <c r="A114" s="4" t="s">
         <v>106</v>
       </c>
@@ -2385,7 +1897,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="115" customHeight="1" ht="18">
       <c r="A115" s="4" t="s">
         <v>106</v>
       </c>
@@ -2393,7 +1905,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="116" customHeight="1" ht="18">
       <c r="A116" s="4" t="s">
         <v>106</v>
       </c>
@@ -2401,7 +1913,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="117" customHeight="1" ht="18">
       <c r="A117" s="4" t="s">
         <v>106</v>
       </c>
@@ -2409,7 +1921,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="118" customHeight="1" ht="18">
       <c r="A118" s="4" t="s">
         <v>106</v>
       </c>
@@ -2417,7 +1929,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="119" customHeight="1" ht="18">
       <c r="A119" s="4" t="s">
         <v>106</v>
       </c>
@@ -2425,7 +1937,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="120" customHeight="1" ht="18">
       <c r="A120" s="4" t="s">
         <v>106</v>
       </c>
@@ -2433,7 +1945,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="121" customHeight="1" ht="18">
       <c r="A121" s="4" t="s">
         <v>106</v>
       </c>
@@ -2441,7 +1953,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="122" customHeight="1" ht="18">
       <c r="A122" s="4" t="s">
         <v>106</v>
       </c>
@@ -2449,7 +1961,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="123" customHeight="1" ht="18">
       <c r="A123" s="4" t="s">
         <v>106</v>
       </c>
@@ -2457,7 +1969,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="124" customHeight="1" ht="18">
       <c r="A124" s="4" t="s">
         <v>106</v>
       </c>
@@ -2465,7 +1977,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="125" customHeight="1" ht="18">
       <c r="A125" s="4" t="s">
         <v>106</v>
       </c>
@@ -2473,7 +1985,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="126" customHeight="1" ht="18">
       <c r="A126" s="4" t="s">
         <v>106</v>
       </c>
@@ -2481,7 +1993,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="127" customHeight="1" ht="18">
       <c r="A127" s="4" t="s">
         <v>106</v>
       </c>
@@ -2489,7 +2001,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="128" customHeight="1" ht="18">
       <c r="A128" s="4" t="s">
         <v>106</v>
       </c>
@@ -2497,7 +2009,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="129" customHeight="1" ht="18">
       <c r="A129" s="7" t="s">
         <v>123</v>
       </c>
@@ -2505,7 +2017,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="130" customHeight="1" ht="18">
       <c r="A130" s="7" t="s">
         <v>123</v>
       </c>
@@ -2513,7 +2025,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="131" customHeight="1" ht="18">
       <c r="A131" s="7" t="s">
         <v>123</v>
       </c>
@@ -2521,7 +2033,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="132" customHeight="1" ht="18">
       <c r="A132" s="7" t="s">
         <v>123</v>
       </c>
@@ -2529,7 +2041,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="133" customHeight="1" ht="18">
       <c r="A133" s="7" t="s">
         <v>123</v>
       </c>
@@ -2537,7 +2049,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="134" customHeight="1" ht="18">
       <c r="A134" s="7" t="s">
         <v>123</v>
       </c>
@@ -2545,7 +2057,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="135" customHeight="1" ht="18">
       <c r="A135" s="7" t="s">
         <v>123</v>
       </c>
@@ -2553,7 +2065,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="136" customHeight="1" ht="18">
       <c r="A136" s="7" t="s">
         <v>123</v>
       </c>
@@ -2561,7 +2073,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="137" customHeight="1" ht="18">
       <c r="A137" s="7" t="s">
         <v>123</v>
       </c>
@@ -2569,7 +2081,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="138" customHeight="1" ht="18">
       <c r="A138" s="7" t="s">
         <v>123</v>
       </c>
@@ -2577,7 +2089,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="139" customHeight="1" ht="18">
       <c r="A139" s="7" t="s">
         <v>123</v>
       </c>
@@ -2585,7 +2097,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="140" customHeight="1" ht="18">
       <c r="A140" s="7" t="s">
         <v>123</v>
       </c>
@@ -2593,7 +2105,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="141" customHeight="1" ht="18">
       <c r="A141" s="7" t="s">
         <v>123</v>
       </c>
@@ -2601,7 +2113,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="142" customHeight="1" ht="18">
       <c r="A142" s="7" t="s">
         <v>123</v>
       </c>
@@ -2609,7 +2121,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="143" customHeight="1" ht="18">
       <c r="A143" s="8" t="s">
         <v>138</v>
       </c>
@@ -2617,7 +2129,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="144" customHeight="1" ht="18">
       <c r="A144" s="8" t="s">
         <v>138</v>
       </c>
@@ -2625,7 +2137,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="145" customHeight="1" ht="18">
       <c r="A145" s="8" t="s">
         <v>138</v>
       </c>
@@ -2633,7 +2145,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="146" customHeight="1" ht="18">
       <c r="A146" s="8" t="s">
         <v>138</v>
       </c>
@@ -2641,7 +2153,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="147" customHeight="1" ht="18">
       <c r="A147" s="8" t="s">
         <v>138</v>
       </c>
@@ -2649,7 +2161,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="148" customHeight="1" ht="18">
       <c r="A148" s="8" t="s">
         <v>138</v>
       </c>
@@ -2657,7 +2169,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="149" customHeight="1" ht="18">
       <c r="A149" s="8" t="s">
         <v>138</v>
       </c>
@@ -2665,7 +2177,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="150" customHeight="1" ht="18">
       <c r="A150" s="8" t="s">
         <v>138</v>
       </c>
@@ -2673,7 +2185,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="151" customHeight="1" ht="18">
       <c r="A151" s="8" t="s">
         <v>138</v>
       </c>
@@ -2681,7 +2193,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="152" customHeight="1" ht="18">
       <c r="A152" s="8" t="s">
         <v>138</v>
       </c>
@@ -2689,7 +2201,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="153" customHeight="1" ht="18">
       <c r="A153" s="8" t="s">
         <v>138</v>
       </c>
@@ -2697,7 +2209,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="154" customHeight="1" ht="18">
       <c r="A154" s="8" t="s">
         <v>138</v>
       </c>
@@ -2705,7 +2217,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="155" customHeight="1" ht="18">
       <c r="A155" s="8" t="s">
         <v>138</v>
       </c>
@@ -2713,7 +2225,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="156" customHeight="1" ht="18">
       <c r="A156" s="8" t="s">
         <v>138</v>
       </c>
@@ -2721,7 +2233,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="157" customHeight="1" ht="18">
       <c r="A157" s="8" t="s">
         <v>138</v>
       </c>
@@ -2729,7 +2241,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="158" customHeight="1" ht="18">
       <c r="A158" s="8" t="s">
         <v>138</v>
       </c>
@@ -2737,7 +2249,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="159" customHeight="1" ht="18">
       <c r="A159" s="8" t="s">
         <v>138</v>
       </c>
@@ -2745,7 +2257,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="160" customHeight="1" ht="18">
       <c r="A160" s="8" t="s">
         <v>138</v>
       </c>
@@ -2753,7 +2265,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="161" customHeight="1" ht="18">
       <c r="A161" s="8" t="s">
         <v>138</v>
       </c>
@@ -2761,7 +2273,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="162" customHeight="1" ht="18">
       <c r="A162" s="8" t="s">
         <v>138</v>
       </c>
@@ -2769,7 +2281,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="163" customHeight="1" ht="18">
       <c r="A163" s="8" t="s">
         <v>138</v>
       </c>
@@ -2777,7 +2289,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="164" customHeight="1" ht="18">
       <c r="A164" s="8" t="s">
         <v>138</v>
       </c>
@@ -2785,7 +2297,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="165" customHeight="1" ht="18">
       <c r="A165" s="8" t="s">
         <v>138</v>
       </c>
@@ -2793,7 +2305,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="166" customHeight="1" ht="18">
       <c r="A166" s="8" t="s">
         <v>138</v>
       </c>
@@ -2801,7 +2313,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="167" customHeight="1" ht="18">
       <c r="A167" s="8" t="s">
         <v>138</v>
       </c>
@@ -2809,7 +2321,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="168" customHeight="1" ht="18">
       <c r="A168" s="8" t="s">
         <v>138</v>
       </c>
@@ -2817,7 +2329,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="169" customHeight="1" ht="18">
       <c r="A169" s="8" t="s">
         <v>138</v>
       </c>
@@ -2825,7 +2337,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="170" customHeight="1" ht="18">
       <c r="A170" s="8" t="s">
         <v>138</v>
       </c>
@@ -2833,7 +2345,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="171" customHeight="1" ht="18">
       <c r="A171" s="8" t="s">
         <v>138</v>
       </c>
@@ -2841,7 +2353,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="172" customHeight="1" ht="18">
       <c r="A172" s="8" t="s">
         <v>138</v>
       </c>
@@ -2849,7 +2361,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="173" customHeight="1" ht="18">
       <c r="A173" s="8" t="s">
         <v>138</v>
       </c>
@@ -2857,7 +2369,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="174" customHeight="1" ht="18">
       <c r="A174" s="8" t="s">
         <v>138</v>
       </c>
@@ -2865,7 +2377,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="175" customHeight="1" ht="18">
       <c r="A175" s="8" t="s">
         <v>138</v>
       </c>
@@ -2873,7 +2385,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="176" customHeight="1" ht="18">
       <c r="A176" s="8" t="s">
         <v>138</v>
       </c>
@@ -2881,7 +2393,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="177" customHeight="1" ht="18">
       <c r="A177" s="8" t="s">
         <v>138</v>
       </c>
@@ -2889,7 +2401,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="178" customHeight="1" ht="18">
       <c r="A178" s="8" t="s">
         <v>138</v>
       </c>
@@ -2897,7 +2409,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="179" customHeight="1" ht="18">
       <c r="A179" s="8" t="s">
         <v>138</v>
       </c>
@@ -2905,7 +2417,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="180" customHeight="1" ht="18">
       <c r="A180" s="8" t="s">
         <v>138</v>
       </c>
@@ -2913,7 +2425,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="181" customHeight="1" ht="18">
       <c r="A181" s="8" t="s">
         <v>138</v>
       </c>
@@ -2921,7 +2433,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="182" customHeight="1" ht="18">
       <c r="A182" s="8" t="s">
         <v>138</v>
       </c>
@@ -2930,7 +2442,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>